<commit_message>
Se monta formato type + name + id + class + placeholder + size + others + required y se documenta forms
</commit_message>
<xml_diff>
--- a/Views/Otros/ControlFomulariosSoccerFile.xlsx
+++ b/Views/Otros/ControlFomulariosSoccerFile.xlsx
@@ -155,12 +155,6 @@
     <t>TimePlayed</t>
   </si>
   <si>
-    <t>Marital_status</t>
-  </si>
-  <si>
-    <t>current_occupation</t>
-  </si>
-  <si>
     <t>Nombre y/o apodo profesional</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>CreacionPefilJugador3</t>
   </si>
   <si>
-    <t>weight</t>
-  </si>
-  <si>
     <t>Height</t>
   </si>
   <si>
@@ -258,6 +249,15 @@
   </si>
   <si>
     <t>CreacionPefilJugador6</t>
+  </si>
+  <si>
+    <t>CurrentOccupation</t>
+  </si>
+  <si>
+    <t>MaritalStatus</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -661,7 +661,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,10 +977,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>41</v>
@@ -997,10 +997,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
@@ -1017,13 +1017,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>14</v>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>14</v>
@@ -1057,13 +1057,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>14</v>
@@ -1072,18 +1072,18 @@
         <v>34</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>14</v>
@@ -1092,18 +1092,18 @@
         <v>34</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>14</v>
@@ -1117,13 +1117,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>14</v>
@@ -1132,24 +1132,24 @@
         <v>34</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>18</v>
@@ -1157,19 +1157,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>18</v>
@@ -1177,19 +1177,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>18</v>
@@ -1197,19 +1197,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>18</v>
@@ -1217,19 +1217,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>18</v>
@@ -1237,19 +1237,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>18</v>
@@ -1257,19 +1257,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>18</v>
@@ -1277,19 +1277,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Continuacion creacion de perfil DT
</commit_message>
<xml_diff>
--- a/Views/Otros/ControlFomulariosSoccerFile.xlsx
+++ b/Views/Otros/ControlFomulariosSoccerFile.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejo\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="78">
   <si>
     <t>FORMULARIOS</t>
   </si>
@@ -315,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -338,24 +333,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,16 +348,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -438,7 +417,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -473,7 +452,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -650,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -660,11 +639,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" style="1" bestFit="1" customWidth="1"/>
@@ -676,24 +655,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -731,7 +710,7 @@
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -751,7 +730,7 @@
       <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -771,7 +750,7 @@
       <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -791,12 +770,12 @@
       <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -808,10 +787,10 @@
       <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -828,10 +807,10 @@
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -848,10 +827,10 @@
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -868,10 +847,10 @@
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -888,10 +867,10 @@
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -908,10 +887,10 @@
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -928,10 +907,10 @@
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -948,10 +927,10 @@
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -968,10 +947,10 @@
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -988,10 +967,10 @@
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1008,10 +987,10 @@
       <c r="D18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1028,10 +1007,10 @@
       <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1048,10 +1027,10 @@
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1068,7 +1047,7 @@
       <c r="D21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -1088,7 +1067,7 @@
       <c r="D22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F22" s="2" t="s">
@@ -1108,10 +1087,10 @@
       <c r="D23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="E23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1128,7 +1107,7 @@
       <c r="D24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -1295,16 +1274,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A33:F33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>